<commit_message>
post w2p2 lecture link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C658BF99-C0E2-D648-80C2-7116D5BA4C4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78AB991-4189-1A49-A8EC-5D03FF57BE80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25900" yWindow="460" windowWidth="33600" windowHeight="18760" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
+    <workbookView xWindow="25900" yWindow="460" windowWidth="33160" windowHeight="18760" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
   <si>
     <t>week</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>https://youtu.be/7JfYrW_P8KU</t>
+  </si>
+  <si>
+    <t>https://youtu.be/iUAUUwJKad0</t>
   </si>
 </sst>
 </file>
@@ -707,7 +710,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
       <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M4" sqref="M4"/>
+      <selection pane="topRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,6 +882,9 @@
       <c r="L5" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="M5" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="1">

</xml_diff>

<commit_message>
link to w3p1 slides
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78AB991-4189-1A49-A8EC-5D03FF57BE80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F246C6-B51D-CC45-A90B-9E892AB8E6FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25900" yWindow="460" windowWidth="33160" windowHeight="18760" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
+    <workbookView xWindow="16660" yWindow="680" windowWidth="33160" windowHeight="18760" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="102">
   <si>
     <t>week</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>https://youtu.be/iUAUUwJKad0</t>
+  </si>
+  <si>
+    <t>w3p1</t>
   </si>
 </sst>
 </file>
@@ -709,8 +712,8 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M5" sqref="M5"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,7 +899,9 @@
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
double backslash instead of single
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeswinehart/Documents/BRT/FunkProg/c3-fp-2021/website-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BD2FD0-610B-DE41-B13B-6583E48FEEF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D92BA0D-A827-1247-ACB8-782C8131C927}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -324,13 +324,13 @@
     <t>Our second lecture on iteration will introduce [**{purrr}**](https://purrr.tidyverse.org) and contrast these functions with the base R versions. The concept of functional programming will also be discussed more explicitly.</t>
   </si>
   <si>
-    <t>The concept of list columns will be introduced and contrasted with the `base::split()`. By the end of this lecture you should be able to fluently nest and unnest data frames and understand why this is such a powerful framework. The last 20 minutes will be devoted to an \"in-class\" quiz.</t>
-  </si>
-  <si>
-    <t>Our final lecture on functions, we will discuss what makes a function \"good\" and what makes them fragile. In this spirit, we will create many small functions that build toward a single function. Additionally, we the concept of **non-standard evaluation** will be introduced, which is used prevalently throughout the tidyverse and can make programming with the tidyverse a bit more difficult.</t>
-  </si>
-  <si>
     <t>Your final project is due before midnight.</t>
+  </si>
+  <si>
+    <t>The concept of list columns will be introduced and contrasted with the `base::split()`. By the end of this lecture you should be able to fluently nest and unnest data frames and understand why this is such a powerful framework. The last 20 minutes will be devoted to an \\"in-class\\" quiz.</t>
+  </si>
+  <si>
+    <t>Our final lecture on functions, we will discuss what makes a function \\"good\\" and what makes them fragile. In this spirit, we will create many small functions that build toward a single function. Additionally, we the concept of **non-standard evaluation** will be introduced, which is used prevalently throughout the tidyverse and can make programming with the tidyverse a bit more difficult.</t>
   </si>
 </sst>
 </file>
@@ -711,9 +711,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E22" sqref="E22"/>
+      <selection pane="topRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -985,7 +985,7 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>79</v>
@@ -1133,7 +1133,7 @@
         <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>22</v>
@@ -1293,7 +1293,7 @@
         <v>15</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
post w3p1 video link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B46080-AFCF-C546-B324-6EE3FC095BE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A8E6CC-B4AE-9540-9CA9-95D196C1E41B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
   <si>
     <t>week</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>w4p1</t>
+  </si>
+  <si>
+    <t>https://youtu.be/pPQrLBPjHPc</t>
   </si>
 </sst>
 </file>
@@ -714,9 +717,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,6 +911,9 @@
       <c r="E6" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="M6" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="1">

</xml_diff>

<commit_message>
draft of w5 slides
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A8E6CC-B4AE-9540-9CA9-95D196C1E41B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B722DB-DB42-AD4A-A168-0789A0E82232}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
+    <workbookView xWindow="16700" yWindow="600" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
   <si>
     <t>week</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t>https://youtu.be/pPQrLBPjHPc</t>
+  </si>
+  <si>
+    <t>w4p2</t>
+  </si>
+  <si>
+    <t>w5p1</t>
+  </si>
+  <si>
+    <t>w5p2</t>
   </si>
 </sst>
 </file>
@@ -717,9 +726,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -994,7 +1003,9 @@
       <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>100</v>
       </c>
@@ -1031,7 +1042,9 @@
       <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>49</v>
       </c>
@@ -1045,6 +1058,9 @@
       </c>
       <c r="C11" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
w6 slides and update PDFs
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501BA6F3-7C81-774E-9C02-5024E29B5864}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97D5C88-A84E-2347-9B87-9983E1E38EB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16700" yWindow="600" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
   <si>
     <t>week</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>https://youtu.be/OiVIV_IWkYw</t>
+  </si>
+  <si>
+    <t>w6p1</t>
+  </si>
+  <si>
+    <t>w6p2</t>
   </si>
 </sst>
 </file>
@@ -738,9 +744,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1095,7 +1101,9 @@
       <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>51</v>
       </c>
@@ -1116,6 +1124,9 @@
       </c>
       <c r="C13" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
video and slide links
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97D5C88-A84E-2347-9B87-9983E1E38EB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AF9810-3639-B548-B375-C18C2E22F925}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16700" yWindow="600" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="114">
   <si>
     <t>week</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>w6p2</t>
+  </si>
+  <si>
+    <t>https://youtu.be/BQ7PX5AAA4Y</t>
   </si>
 </sst>
 </file>
@@ -744,9 +747,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1090,6 +1093,9 @@
       <c r="E11" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="M11" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1">

</xml_diff>

<commit_message>
fix slides, add w7p2 slide link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352F47CB-0E25-9845-BB12-FD6F3E5F85C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DFFEBC-B7A8-DD49-BA87-2C196D791B2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16700" yWindow="600" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -756,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D16" sqref="D16"/>
     </sheetView>

</xml_diff>

<commit_message>
Add w7 lecture video
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73C6F95-3BE6-BD4F-8BF2-4E7632D9FBA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D25342-9357-E640-8951-D6A531F94127}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16700" yWindow="600" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
+    <workbookView xWindow="4800" yWindow="600" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="119">
   <si>
     <t>week</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>https://youtu.be/E6koeYBK3JA</t>
+  </si>
+  <si>
+    <t>https://youtu.be/rV9QMh0wBcw</t>
   </si>
 </sst>
 </file>
@@ -761,7 +764,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
       <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M13" sqref="M13"/>
+      <selection pane="topRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1199,7 +1202,9 @@
       <c r="L14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M14" s="6"/>
+      <c r="M14" s="6" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" s="1">

</xml_diff>

<commit_message>
w8 slides (and w7p2 video)
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D25342-9357-E640-8951-D6A531F94127}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0911521E-0A91-2340-A411-D534836DBC4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="600" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="121">
   <si>
     <t>week</t>
   </si>
@@ -382,6 +382,12 @@
   </si>
   <si>
     <t>https://youtu.be/rV9QMh0wBcw</t>
+  </si>
+  <si>
+    <t>https://youtu.be/JrhBTl4EROQ</t>
+  </si>
+  <si>
+    <t>w8p1</t>
   </si>
 </sst>
 </file>
@@ -762,9 +768,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1228,7 +1234,9 @@
       <c r="K15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M15" s="6"/>
+      <c r="M15" s="6" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1239,6 +1247,9 @@
       </c>
       <c r="C16" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Post w9p2 video link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2020-21/c3-fp-2021/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F173B7-3A4C-7340-B317-1D85060977B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58792686-709C-2E43-B8EE-99198C1D70B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="600" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="129">
   <si>
     <t>week</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>w10p2</t>
+  </si>
+  <si>
+    <t>https://youtu.be/sRSwCdN7ZlI</t>
   </si>
 </sst>
 </file>
@@ -790,8 +793,8 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D21" sqref="D21"/>
+      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1384,6 +1387,9 @@
       <c r="K19" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="M19" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">

</xml_diff>